<commit_message>
menambahkan logika sheet billing
</commit_message>
<xml_diff>
--- a/hasil/output.xlsx
+++ b/hasil/output.xlsx
@@ -9,7 +9,9 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Daily" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Monthly" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weekly" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Monthly" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Billing" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,121 +425,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ih_telomanys_customers</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TABLE NAME</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>EVENT DATE</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>DATE TRANSACTION</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>DATE AVAILABILITY</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NOW SIZE CONDITION</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ih_telomanys_customers</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>event_date=2024-11-05</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2024-11-06</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>04:50</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>36.6 K</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ih_telomanys_customers</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>event_date=2024-11-08</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2024-11-09</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>04:50</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>24.1 K</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ih_telomanys_customers</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>event_date=2024-11-14</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2024-11-15</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>04:49</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>21.9 K</t>
-        </is>
-      </c>
-    </row>
+    <row r="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3623,6 +3511,140 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ih_telomanys_customers</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TABLE NAME</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>EVENT DATE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DATE TRANSACTION</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>DATE AVAILABILITY</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NOW SIZE CONDITION</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ih_telomanys_customers</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>event_date=2024-11-05</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-11-06</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>04:50</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>36.6 K</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ih_telomanys_customers</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>event_date=2024-11-08</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-11-09</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>04:50</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>24.1 K</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ih_telomanys_customers</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>event_date=2024-11-14</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-11-15</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>04:49</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>21.9 K</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3819,4 +3841,84 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ih_biling_ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TABLE NAME</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>EVENT DATE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DATE TRANSACTION</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>DATE AVAILABILITY</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NOW SIZE CONDITION</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ih_biling_ih</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>event_date=2024-11-05</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-11-06</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>04:50</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>36.6 K</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>